<commit_message>
Uploaded newest version of Beslutstabell
</commit_message>
<xml_diff>
--- a/Beslutstabell Attackering.xlsx
+++ b/Beslutstabell Attackering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\inte_projektarbete_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1642D774-0201-4F70-AAA6-62BEE8633A15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577595D8-852F-4AA3-8300-0CB676D28AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{040C2F1F-8940-4EF1-A5C6-D16244747B0C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="61">
   <si>
     <t>Anfallaren är död</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>En anfallare med 5 livspoäng och 2 attackstyrka skapas som ska attackera en motståndare med 5 livspoäng som är svag mot is med en avståndsisattack.</t>
+  </si>
+  <si>
+    <t>En anfallare med 5 livspoäng och 2 attackstyrka skapas som ska attackera en motståndare med 5 livspoäng som är resistant mot fysiska attacker med en fysiskattack.</t>
   </si>
 </sst>
 </file>
@@ -763,7 +766,7 @@
   <dimension ref="A1:T32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1623,7 @@
         <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="T31" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
moved some test methods
</commit_message>
<xml_diff>
--- a/Beslutstabell Attackering.xlsx
+++ b/Beslutstabell Attackering.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\inte_projektarbete_final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577595D8-852F-4AA3-8300-0CB676D28AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F86B666-871B-4D38-A10D-9E53320368C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{040C2F1F-8940-4EF1-A5C6-D16244747B0C}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>Testfall</t>
   </si>
   <si>
-    <t>Vilkor</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>En anfallare med 5 livspoäng och 2 attackstyrka skapas som ska attackera en motståndare med 5 livspoäng som är resistant mot fysiska attacker med en fysiskattack.</t>
+  </si>
+  <si>
+    <t>Villkor</t>
   </si>
 </sst>
 </file>
@@ -289,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -388,6 +388,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -396,7 +436,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -428,12 +468,22 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Beräkning" xfId="4" builtinId="22"/>
@@ -763,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55145D2B-1B18-4B67-9C80-5B65FD69CDCE}">
-  <dimension ref="A1:T32"/>
+  <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,66 +827,66 @@
     <col min="4" max="4" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -895,7 +945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -954,7 +1004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +1063,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1072,7 +1122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1131,7 +1181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1190,7 +1240,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1249,7 +1299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1308,7 +1358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1367,7 +1417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1377,16 +1427,16 @@
       <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>0</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <v>0</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="11">
         <v>0</v>
       </c>
       <c r="H11" s="5" t="s">
@@ -1426,219 +1476,301 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>20</v>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15"/>
+      <c r="W13" s="15"/>
+      <c r="X13" s="15"/>
+      <c r="Y13" s="15"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="S14" s="12"/>
       <c r="T14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>21</v>
+      <c r="Y14" s="18"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="S15" s="12"/>
       <c r="T15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="Y15" s="12"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="S16" s="12"/>
+      <c r="T16" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y16" s="12"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="S17" s="12"/>
+      <c r="T17" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y17" s="12"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="S18" s="12"/>
+      <c r="T18" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y18" s="12"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="S19" s="12"/>
+      <c r="T19" t="s">
         <v>42</v>
       </c>
-      <c r="T16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="T17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="Y19" s="12"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
         <v>45</v>
       </c>
-      <c r="T18" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
-      <c r="T19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="S20" s="12"/>
+      <c r="T20" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y20" s="12"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="S21" s="12"/>
+      <c r="T21" t="s">
         <v>46</v>
       </c>
-      <c r="T20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="Y21" s="12"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>48</v>
       </c>
-      <c r="T21" t="s">
+      <c r="S22" s="12"/>
+      <c r="T22" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y22" s="12"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="S23" s="12"/>
+      <c r="T23" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y23" s="12"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>52</v>
+      </c>
+      <c r="S24" s="12"/>
+      <c r="T24" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y24" s="12"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="S25" s="12"/>
+      <c r="T25" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y25" s="12"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="S26" s="12"/>
+      <c r="T26" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y26" s="12"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+      <c r="S27" s="12"/>
+      <c r="T27" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y27" s="12"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="S28" s="12"/>
+      <c r="T28" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y28" s="12"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="S29" s="12"/>
+      <c r="T29" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y29" s="12"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="S30" s="12"/>
+      <c r="T30" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y30" s="12"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>59</v>
+      </c>
+      <c r="S31" s="12"/>
+      <c r="T31" t="s">
         <v>49</v>
       </c>
-      <c r="T22" t="s">
+      <c r="Y31" s="12"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
-      <c r="T23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" t="s">
-        <v>53</v>
-      </c>
-      <c r="T24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" t="s">
-        <v>52</v>
-      </c>
-      <c r="T25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
-      <c r="T26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
-      <c r="T27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" t="s">
-        <v>57</v>
-      </c>
-      <c r="T28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" t="s">
-        <v>59</v>
-      </c>
-      <c r="T29" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" t="s">
-        <v>48</v>
-      </c>
-      <c r="T30" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" t="s">
-        <v>60</v>
-      </c>
-      <c r="T31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" t="s">
-        <v>58</v>
-      </c>
-      <c r="T32" t="s">
-        <v>51</v>
-      </c>
+      <c r="U32" s="15"/>
+      <c r="V32" s="15"/>
+      <c r="W32" s="15"/>
+      <c r="X32" s="15"/>
+      <c r="Y32" s="17"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="N7:S7">

</xml_diff>